<commit_message>
json data 4 nov
</commit_message>
<xml_diff>
--- a/timesheets/2020_timebook.xlsx
+++ b/timesheets/2020_timebook.xlsx
@@ -1,13 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="14790" yWindow="2205" windowWidth="12885" windowHeight="11505" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Template" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="August" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Template" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="August" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="November" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="191029" fullCalcOnLoad="1"/>
@@ -428,7 +429,7 @@
       <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="10.5703125" bestFit="1" customWidth="1" style="1" min="1" max="1"/>
     <col width="22" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
@@ -554,7 +555,7 @@
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="17" customWidth="1" style="1" min="1" max="1"/>
     <col width="48" customWidth="1" style="1" min="2" max="2"/>
@@ -648,4 +649,81 @@
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>TIMESHEET</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>CNR</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>.Architects</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>MONTH:</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>xxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>NAME:</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>xxx</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>PROJECT</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>DESCRIPTION OF WORK</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>OFFICE USE</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
json data 5 nov
</commit_message>
<xml_diff>
--- a/timesheets/2020_timebook.xlsx
+++ b/timesheets/2020_timebook.xlsx
@@ -657,26 +657,31 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="17" customWidth="1" style="1" min="1" max="1"/>
+    <col width="48" customWidth="1" style="1" min="2" max="2"/>
+    <col width="17" customWidth="1" style="1" min="3" max="3"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="4" t="inlineStr">
         <is>
           <t>TIMESHEET</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t>CNR</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
+      <c r="B1" s="5" t="inlineStr">
+        <is>
+          <t>cnr</t>
+        </is>
+      </c>
+      <c r="C1" s="6" t="inlineStr">
         <is>
           <t>.Architects</t>
         </is>
@@ -690,7 +695,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>xxx</t>
+          <t>November 2020</t>
         </is>
       </c>
     </row>
@@ -702,24 +707,50 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>xxx</t>
+          <t>tertert</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="7" t="inlineStr">
         <is>
           <t>PROJECT</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="B6" s="7" t="inlineStr">
         <is>
           <t>DESCRIPTION OF WORK</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+      <c r="C6" s="7" t="inlineStr">
         <is>
           <t>OFFICE USE</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>Week1</t>
+        </is>
+      </c>
+      <c r="B7" s="8" t="n"/>
+      <c r="C7" s="8" t="n"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="8" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="B8" s="8" t="inlineStr">
+        <is>
+          <t>rggergergr</t>
+        </is>
+      </c>
+      <c r="C8" s="8" t="inlineStr">
+        <is>
+          <t>*</t>
         </is>
       </c>
     </row>

</xml_diff>